<commit_message>
10 line test file
</commit_message>
<xml_diff>
--- a/web/templates/canada_covid19/exampleInput/canCOGeN-validTestData_3-0-0.xlsx
+++ b/web/templates/canada_covid19/exampleInput/canCOGeN-validTestData_3-0-0.xlsx
@@ -1296,7 +1296,7 @@
         <v/>
       </c>
       <c r="EM3" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="4">
@@ -1727,7 +1727,7 @@
         <v/>
       </c>
       <c r="EM4" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="5">
@@ -2158,7 +2158,7 @@
         <v/>
       </c>
       <c r="EM5" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="6">
@@ -2589,7 +2589,7 @@
         <v/>
       </c>
       <c r="EM6" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="7">
@@ -3020,7 +3020,7 @@
         <v/>
       </c>
       <c r="EM7" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="8">
@@ -3451,7 +3451,7 @@
         <v/>
       </c>
       <c r="EM8" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="9">
@@ -3882,7 +3882,7 @@
         <v/>
       </c>
       <c r="EM9" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="10">
@@ -4313,7 +4313,7 @@
         <v/>
       </c>
       <c r="EM10" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="11">
@@ -4744,7 +4744,7 @@
         <v/>
       </c>
       <c r="EM11" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="12">
@@ -5175,7 +5175,7 @@
         <v/>
       </c>
       <c r="EM12" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="13">
@@ -5606,7 +5606,7 @@
         <v/>
       </c>
       <c r="EM13" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="14">
@@ -6037,7 +6037,7 @@
         <v/>
       </c>
       <c r="EM14" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="15">
@@ -6078,7 +6078,7 @@
         <v/>
       </c>
       <c r="M15" t="str">
-        <v>St. Joseph’s Healthcare Hamilton</v>
+        <v>St. Joseph's Healthcare Hamilton</v>
       </c>
       <c r="N15" t="str">
         <v/>
@@ -6468,7 +6468,7 @@
         <v/>
       </c>
       <c r="EM15" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
     <row r="16">
@@ -6509,7 +6509,7 @@
         <v/>
       </c>
       <c r="M16" t="str">
-        <v>St. Joseph’s Healthcare Hamilton</v>
+        <v>St. Joseph's Healthcare Hamilton</v>
       </c>
       <c r="N16" t="str">
         <v/>
@@ -6899,7 +6899,7 @@
         <v/>
       </c>
       <c r="EM16" t="str">
-        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v2.4.1</v>
+        <v>DataHarmonizer v1.9.0, CanCOGeNCovid19 v3.0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>